<commit_message>
updated cities in comedian spreadsheet and added commedians to the seed file
</commit_message>
<xml_diff>
--- a/list of comedians.xlsx
+++ b/list of comedians.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/earltstephens/turing/1811_2module/projects/LaughTracks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A1D140-8B7D-D14A-BC4C-EDE781B470A1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A9BE14-C35E-DA48-8145-BBE9814F45A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2900" yWindow="10660" windowWidth="28040" windowHeight="10340" xr2:uid="{911CAA23-51BE-0A4B-B1E6-3F108DD47651}"/>
+    <workbookView xWindow="2140" yWindow="15160" windowWidth="19880" windowHeight="10340" xr2:uid="{911CAA23-51BE-0A4B-B1E6-3F108DD47651}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,14 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
   <si>
     <t>Ellen DeGeneres</t>
   </si>
   <si>
-    <t>Los Angeles</t>
-  </si>
-  <si>
     <t>Ellen DeGeneres: Relatable</t>
   </si>
   <si>
@@ -81,9 +78,6 @@
     <t>https://m.media-amazon.com/images/M/MV5BMTk5MDE5NDcxOV5BMl5BanBnXkFtZTcwNTAxOTkwMg@@._V1_UY317_CR12,0,214,317_AL_.jpg</t>
   </si>
   <si>
-    <t>Carol Burness</t>
-  </si>
-  <si>
     <t>https://m.media-amazon.com/images/M/MV5BNjE2OTQxODkyMV5BMl5BanBnXkFtZTYwODM5MzQz._V1_UY98_CR2,0,67,98_AL_.jpg</t>
   </si>
   <si>
@@ -156,9 +150,6 @@
     <t>Chris Rock</t>
   </si>
   <si>
-    <t>Alpine</t>
-  </si>
-  <si>
     <t>https://m.media-amazon.com/images/M/MV5BMTEyNjM5MjgyNzdeQTJeQWpwZ15BbWU3MDAzMzUyODc@._V1.._UX214_CR0,0,214,317_AL_.jpg</t>
   </si>
   <si>
@@ -201,9 +192,6 @@
     <t>Larry the Cable Guy</t>
   </si>
   <si>
-    <t>Lincoln</t>
-  </si>
-  <si>
     <t>https://m.media-amazon.com/images/M/MV5BMTY5MjA0MjQ4Ml5BMl5BanBnXkFtZTcwNTIwMTc2NQ@@._V1_UY317_CR10,0,214,317_AL_.jpg</t>
   </si>
   <si>
@@ -222,9 +210,6 @@
     <t>Eddie Murphy</t>
   </si>
   <si>
-    <t>Beverly Hills</t>
-  </si>
-  <si>
     <t>https://www.imdb.com/name/nm0000552/mediaviewer/rm803183360?ref_=nm_ov_ph</t>
   </si>
   <si>
@@ -276,7 +261,43 @@
     <t>https://m.media-amazon.com/images/M/MV5BZWJlMzAxMGItNzRlMS00MTIzLTljMzItMDI5ZjIxYzU5ZTIyXkEyXkFqcGdeQXVyNjYzMDA4MTI@._V1_UY268_CR4,0,182,268_AL_.jpg</t>
   </si>
   <si>
-    <t>Mill Valley</t>
+    <t>Metairie</t>
+  </si>
+  <si>
+    <t>San Jose</t>
+  </si>
+  <si>
+    <t>Portsmouth</t>
+  </si>
+  <si>
+    <t>Oak Park</t>
+  </si>
+  <si>
+    <t>Carol Burnett</t>
+  </si>
+  <si>
+    <t>San Antonio</t>
+  </si>
+  <si>
+    <t>West Germany</t>
+  </si>
+  <si>
+    <t>Andrews</t>
+  </si>
+  <si>
+    <t>Fritch</t>
+  </si>
+  <si>
+    <t>Pawnee City</t>
+  </si>
+  <si>
+    <t>Brooklyn</t>
+  </si>
+  <si>
+    <t>Denver</t>
+  </si>
+  <si>
+    <t>Missoula</t>
   </si>
 </sst>
 </file>
@@ -641,8 +662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92E53E98-9E41-8F40-87D5-402FF644F4AF}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -662,126 +683,126 @@
         <v>61</v>
       </c>
       <c r="C1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
       </c>
       <c r="F1">
         <v>68</v>
       </c>
       <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
         <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F2">
         <v>60</v>
       </c>
       <c r="G2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F3">
         <v>66</v>
       </c>
       <c r="G3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4">
         <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4">
         <v>75</v>
       </c>
       <c r="G4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F5">
         <v>90</v>
       </c>
       <c r="G5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6">
         <v>54</v>
       </c>
       <c r="C6" t="s">
-        <v>1</v>
+        <v>80</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F6">
         <v>87</v>
       </c>
       <c r="G6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F7">
         <v>59</v>
       </c>
       <c r="G7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8">
         <v>89</v>
       </c>
       <c r="C8" t="s">
-        <v>1</v>
+        <v>81</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F8">
         <v>60</v>
@@ -789,323 +810,324 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F9">
         <v>60</v>
       </c>
       <c r="G9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>82</v>
       </c>
       <c r="B10">
         <v>85</v>
       </c>
       <c r="C10" t="s">
-        <v>1</v>
+        <v>83</v>
       </c>
       <c r="D10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F10">
         <v>120</v>
       </c>
       <c r="G10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F11">
         <v>60</v>
       </c>
       <c r="G11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F12">
         <v>88</v>
       </c>
       <c r="G12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B13">
         <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>1</v>
+        <v>84</v>
       </c>
       <c r="D13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" t="s">
         <v>35</v>
-      </c>
-      <c r="E13" t="s">
-        <v>37</v>
       </c>
       <c r="F13">
         <v>60</v>
       </c>
       <c r="G13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F14">
         <v>62</v>
       </c>
       <c r="G14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F15">
         <v>60</v>
       </c>
       <c r="G15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B16">
         <v>53</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>85</v>
       </c>
       <c r="D16" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E16" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F16">
         <v>27</v>
       </c>
       <c r="G16" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E17" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F17">
         <v>65</v>
       </c>
       <c r="G17" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E18" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F18">
         <v>80</v>
       </c>
       <c r="G18" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B19">
         <v>62</v>
       </c>
       <c r="C19" t="s">
-        <v>1</v>
+        <v>86</v>
       </c>
       <c r="D19" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E19" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F19">
         <v>63</v>
       </c>
       <c r="G19" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E20" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F20">
         <v>76</v>
       </c>
       <c r="G20" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B21">
         <v>55</v>
       </c>
       <c r="C21" t="s">
-        <v>58</v>
-      </c>
-      <c r="D21" t="s">
-        <v>59</v>
+        <v>87</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="E21" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F21">
         <v>75</v>
       </c>
       <c r="G21" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E22" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F22">
         <v>90</v>
       </c>
       <c r="G22" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B23">
         <v>57</v>
       </c>
       <c r="C23" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="D23" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E23" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F23">
         <v>69</v>
       </c>
       <c r="G23" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E24" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="F24">
         <v>93</v>
       </c>
       <c r="G24" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B25">
         <v>65</v>
       </c>
       <c r="C25" t="s">
-        <v>1</v>
+        <v>89</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E25" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F25">
         <v>30</v>
       </c>
       <c r="G25" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E26" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F26">
         <v>30</v>
       </c>
       <c r="G26" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B27">
         <v>63</v>
       </c>
       <c r="C27" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="D27" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E27" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F27">
         <v>56</v>
       </c>
       <c r="G27" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E28" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F28">
         <v>64</v>
       </c>
       <c r="G28" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D25" r:id="rId1" xr:uid="{D4849A08-ED2C-7448-AD4B-F72F5152BB0C}"/>
+    <hyperlink ref="D21" r:id="rId2" xr:uid="{A8C95C7A-9DE3-E649-A580-67B8BBA8C970}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated seed file with specials and ran rake db seed
</commit_message>
<xml_diff>
--- a/list of comedians.xlsx
+++ b/list of comedians.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/earltstephens/turing/1811_2module/projects/LaughTracks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A9BE14-C35E-DA48-8145-BBE9814F45A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E1D15C-1B35-AD41-9AF3-1B1116AF5000}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2140" yWindow="15160" windowWidth="19880" windowHeight="10340" xr2:uid="{911CAA23-51BE-0A4B-B1E6-3F108DD47651}"/>
+    <workbookView xWindow="1560" yWindow="13220" windowWidth="29440" windowHeight="10340" xr2:uid="{911CAA23-51BE-0A4B-B1E6-3F108DD47651}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -662,8 +662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92E53E98-9E41-8F40-87D5-402FF644F4AF}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>